<commit_message>
update DB design file
</commit_message>
<xml_diff>
--- a/src/main/resources/DB.xlsx
+++ b/src/main/resources/DB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94">
   <si>
     <t>NO</t>
   </si>
@@ -278,6 +278,24 @@
   </si>
   <si>
     <t>报名者踢球的位置</t>
+  </si>
+  <si>
+    <t>T_DICTIONARY</t>
+  </si>
+  <si>
+    <t>D_ID</t>
+  </si>
+  <si>
+    <t>D_NAMME</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <t>D_TYPE</t>
+  </si>
+  <si>
+    <t>类型</t>
   </si>
 </sst>
 </file>
@@ -736,10 +754,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1902,7 +1920,7 @@
         <v>86</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5" t="s">
@@ -1910,44 +1928,40 @@
       </c>
       <c r="E82" s="1" t="str">
         <f>A82&amp;" "&amp;B82&amp;" "&amp;C82&amp;", "</f>
-        <v>MATCH_MEMBER_POSITION DATE , </v>
+        <v>MATCH_MEMBER_POSITION VARCHAR(100) , </v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="5" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C83" s="5"/>
-      <c r="D83" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="D83" s="6"/>
       <c r="E83" s="1" t="str">
         <f>A83&amp;" "&amp;B83&amp;" "&amp;C83&amp;", "</f>
-        <v>MATCH_ADDRESS VARCHAR(500) , </v>
+        <v>INPUT_NAME VARCHAR(100) , </v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="5" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C84" s="5"/>
-      <c r="D84" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="D84" s="6"/>
       <c r="E84" s="1" t="str">
         <f>A84&amp;" "&amp;B84&amp;" "&amp;C84&amp;", "</f>
-        <v>MATCH_ORGANIZER DECIMAL(10,0) , </v>
+        <v>INPUT_DATE DATE , </v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>14</v>
@@ -1956,12 +1970,12 @@
       <c r="D85" s="6"/>
       <c r="E85" s="1" t="str">
         <f>A85&amp;" "&amp;B85&amp;" "&amp;C85&amp;", "</f>
-        <v>INPUT_NAME VARCHAR(100) , </v>
+        <v>UPDATE_NAME VARCHAR(100) , </v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>1</v>
@@ -1970,50 +1984,198 @@
       <c r="D86" s="6"/>
       <c r="E86" s="1" t="str">
         <f>A86&amp;" "&amp;B86&amp;" "&amp;C86&amp;", "</f>
-        <v>INPUT_DATE DATE , </v>
+        <v>UPDATE_DATE DATE , </v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C87" s="5"/>
-      <c r="D87" s="6"/>
+      <c r="D87" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E87" s="1" t="str">
         <f>A87&amp;" "&amp;B87&amp;" "&amp;C87&amp;", "</f>
+        <v>DELSIGN DECIMAL(1,0) , </v>
+      </c>
+    </row>
+    <row r="89" ht="18.75" spans="1:4">
+      <c r="A89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="3">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" s="4">
+        <v>42269</v>
+      </c>
+    </row>
+    <row r="90" ht="18.75" spans="1:4">
+      <c r="A90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" ht="18.75" spans="1:5">
+      <c r="A91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="1" t="str">
+        <f>"drop table "&amp;B90&amp;";"</f>
+        <v>drop table T_DICTIONARY;</v>
+      </c>
+    </row>
+    <row r="92" ht="18.75" spans="1:5">
+      <c r="A92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="1" t="str">
+        <f>"create table "&amp;B90&amp;" ("</f>
+        <v>create table T_DICTIONARY (</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="5"/>
+      <c r="E93" s="1" t="str">
+        <f>A93&amp;" "&amp;B93&amp;" "&amp;C93&amp;", "</f>
+        <v>D_ID DECIMAL(10,0) NOT NULL PRIMARY KEY, </v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="1" t="str">
+        <f>A94&amp;" "&amp;B94&amp;" "&amp;C94&amp;", "</f>
+        <v>D_NAMME VARCHAR(500) , </v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E95" s="1" t="str">
+        <f>A95&amp;" "&amp;B95&amp;" "&amp;C95&amp;", "</f>
+        <v>D_TYPE DECIMAL(10,0) , </v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="1" t="str">
+        <f>A96&amp;" "&amp;B96&amp;" "&amp;C96&amp;", "</f>
+        <v>INPUT_NAME VARCHAR(100) , </v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="1" t="str">
+        <f>A97&amp;" "&amp;B97&amp;" "&amp;C97&amp;", "</f>
+        <v>INPUT_DATE DATE , </v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="1" t="str">
+        <f>A98&amp;" "&amp;B98&amp;" "&amp;C98&amp;", "</f>
         <v>UPDATE_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="5" t="s">
+    <row r="99" spans="1:5">
+      <c r="A99" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B99" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="1" t="str">
-        <f>A88&amp;" "&amp;B88&amp;" "&amp;C88&amp;", "</f>
+      <c r="C99" s="5"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="1" t="str">
+        <f>A99&amp;" "&amp;B99&amp;" "&amp;C99&amp;", "</f>
         <v>UPDATE_DATE DATE , </v>
       </c>
     </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="5" t="s">
+    <row r="100" spans="1:5">
+      <c r="A100" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B100" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5" t="s">
+      <c r="C100" s="5"/>
+      <c r="D100" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E89" s="1" t="str">
-        <f>A89&amp;" "&amp;B89&amp;" "&amp;C89&amp;", "</f>
+      <c r="E100" s="1" t="str">
+        <f>A100&amp;" "&amp;B100&amp;" "&amp;C100&amp;", "</f>
         <v>DELSIGN DECIMAL(1,0) , </v>
       </c>
     </row>

</xml_diff>

<commit_message>
update DB decimal to int
</commit_message>
<xml_diff>
--- a/src/main/resources/DB.xlsx
+++ b/src/main/resources/DB.xlsx
@@ -49,10 +49,10 @@
     <t>ID</t>
   </si>
   <si>
-    <t>DECIMAL(10,0)</t>
-  </si>
-  <si>
-    <t>NOT NULL PRIMARY KEY</t>
+    <t>INT(11)</t>
+  </si>
+  <si>
+    <t>NOT NULL PRIMARY KEY AUTO_INCREMENT</t>
   </si>
   <si>
     <t>用户表非空主键</t>
@@ -127,7 +127,7 @@
     <t>DELSIGN</t>
   </si>
   <si>
-    <t>DECIMAL(1,0)</t>
+    <t>INT(1)</t>
   </si>
   <si>
     <t>删除标识</t>
@@ -348,10 +348,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -801,15 +801,15 @@
   <sheetPr/>
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90:E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="27.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="81.25" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.125" style="1"/>
@@ -886,7 +886,7 @@
       </c>
       <c r="E5" s="1" t="str">
         <f>A5&amp;" "&amp;B5&amp;" "&amp;C5&amp;" comment '"&amp;D5&amp;"' , "</f>
-        <v>ID DECIMAL(10,0) NOT NULL PRIMARY KEY comment '用户表非空主键' , </v>
+        <v>ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '用户表非空主键' , </v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="E16" s="1" t="str">
         <f>A16&amp;" "&amp;B16&amp;" "&amp;C16&amp;" comment '"&amp;D16&amp;"' , "</f>
-        <v>DELSIGN DECIMAL(1,0)  comment '删除标识' , </v>
+        <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="18.75" spans="1:4">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="E22" s="1" t="str">
         <f>A22&amp;" "&amp;B22&amp;" "&amp;C22&amp;" comment '"&amp;D22&amp;"' , "</f>
-        <v>TID DECIMAL(10,0) NOT NULL PRIMARY KEY comment '足球队表非空主键' , </v>
+        <v>TID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球队表非空主键' , </v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:5">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="E26" s="1" t="str">
         <f>A26&amp;" "&amp;B26&amp;" "&amp;C26&amp;" comment '"&amp;D26&amp;"' , "</f>
-        <v>TEAM_CAPTAIN DECIMAL(10,0)  comment '存队长的UID' , </v>
+        <v>TEAM_CAPTAIN INT(11)  comment '存队长的UID' , </v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:5">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="E27" s="1" t="str">
         <f>A27&amp;" "&amp;B27&amp;" "&amp;C27&amp;" comment '"&amp;D27&amp;"' , "</f>
-        <v>TEAM_POINTS DECIMAL(10,0)  comment '球队积分' , </v>
+        <v>TEAM_POINTS INT(11)  comment '球队积分' , </v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" spans="1:5">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="E32" s="1" t="str">
         <f>A32&amp;" "&amp;B32&amp;" "&amp;C32&amp;" comment '"&amp;D32&amp;"' , "</f>
-        <v>DELSIGN DECIMAL(1,0)  comment '删除标识' , </v>
+        <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="18.75" spans="1:4">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="E38" s="1" t="str">
         <f>A38&amp;" "&amp;B38&amp;" "&amp;C38&amp;" comment '"&amp;D38&amp;"' , "</f>
-        <v>TM_ID DECIMAL(10,0) NOT NULL PRIMARY KEY comment '足球队成员表非空主键' , </v>
+        <v>TM_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球队成员表非空主键' , </v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" spans="1:5">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" ref="E39:E50" si="2">A39&amp;" "&amp;B39&amp;" "&amp;C39&amp;" comment '"&amp;D39&amp;"' , "</f>
-        <v>T_ID DECIMAL(10,0)  comment '关联球队TID' , </v>
+        <v>T_ID INT(11)  comment '关联球队TID' , </v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1" spans="1:5">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="E40" s="1" t="str">
         <f>A40&amp;" "&amp;B40&amp;" "&amp;C40&amp;" comment '"&amp;D40&amp;"' , "</f>
-        <v>U_ID DECIMAL(10,0)  comment '用户ID' , </v>
+        <v>U_ID INT(11)  comment '用户ID' , </v>
       </c>
     </row>
     <row r="41" s="1" customFormat="1" spans="1:5">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="E44" s="1" t="str">
         <f>A44&amp;" "&amp;B44&amp;" "&amp;C44&amp;" comment '"&amp;D44&amp;"' , "</f>
-        <v>MEMBER_ABSENT_TIME DECIMAL(10,0)  comment '球员缺席次数' , </v>
+        <v>MEMBER_ABSENT_TIME INT(11)  comment '球员缺席次数' , </v>
       </c>
     </row>
     <row r="45" s="1" customFormat="1" spans="1:5">
@@ -1562,7 +1562,7 @@
       </c>
       <c r="E50" s="1" t="str">
         <f>A50&amp;" "&amp;B50&amp;" "&amp;C50&amp;" comment '"&amp;D50&amp;"' , "</f>
-        <v>DELSIGN DECIMAL(1,0)  comment '删除标识' , </v>
+        <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
     <row r="52" ht="18.75" spans="1:4">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="E56" s="1" t="str">
         <f>A56&amp;" "&amp;B56&amp;" "&amp;C56&amp;" comment '"&amp;D56&amp;"' , "</f>
-        <v>M_ID DECIMAL(10,0) NOT NULL PRIMARY KEY comment '足球比赛表非空主键' , </v>
+        <v>M_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球比赛表非空主键' , </v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="E59" s="1" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59&amp;" comment '"&amp;D59&amp;"' , "</f>
-        <v>MATCH_ORGANIZER DECIMAL(10,0)  comment '组织者UID' , </v>
+        <v>MATCH_ORGANIZER INT(11)  comment '组织者UID' , </v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="E60" s="1" t="str">
         <f>A60&amp;" "&amp;B60&amp;" "&amp;C60&amp;" comment '"&amp;D60&amp;"' , "</f>
-        <v>MATCH_KEEPER_MEMBERS DECIMAL(10,0)  comment '守门员人数' , </v>
+        <v>MATCH_KEEPER_MEMBERS INT(11)  comment '守门员人数' , </v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="E61" s="1" t="str">
         <f>A61&amp;" "&amp;B61&amp;" "&amp;C61&amp;" comment '"&amp;D61&amp;"' , "</f>
-        <v>MATCH_DEFENDER_MEMBERS DECIMAL(10,0)  comment '后卫人数' , </v>
+        <v>MATCH_DEFENDER_MEMBERS INT(11)  comment '后卫人数' , </v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="E62" s="1" t="str">
         <f>A62&amp;" "&amp;B62&amp;" "&amp;C62&amp;" comment '"&amp;D62&amp;"' , "</f>
-        <v>MATCH_MIDFIELDER_MEMBERS DECIMAL(10,0)  comment '中场人数' , </v>
+        <v>MATCH_MIDFIELDER_MEMBERS INT(11)  comment '中场人数' , </v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E63" s="1" t="str">
         <f>A63&amp;" "&amp;B63&amp;" "&amp;C63&amp;" comment '"&amp;D63&amp;"' , "</f>
-        <v>MATCH_STRIKER_MEMBERS DECIMAL(10,0)  comment '前锋人数' , </v>
+        <v>MATCH_STRIKER_MEMBERS INT(11)  comment '前锋人数' , </v>
       </c>
     </row>
     <row r="64" customFormat="1" spans="1:5">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="E64" s="1" t="str">
         <f>A64&amp;" "&amp;B64&amp;" "&amp;C64&amp;" comment '"&amp;D64&amp;"' , "</f>
-        <v>MATCH_REFEREE_MEMBERS DECIMAL(10,0)  comment '裁判人数' , </v>
+        <v>MATCH_REFEREE_MEMBERS INT(11)  comment '裁判人数' , </v>
       </c>
     </row>
     <row r="65" customFormat="1" spans="1:5">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="E65" s="1" t="str">
         <f>A65&amp;" "&amp;B65&amp;" "&amp;C65&amp;" comment '"&amp;D65&amp;"' , "</f>
-        <v>MATCH_TEAMA_ID DECIMAL(10,0)  comment 'A球队临时ID' , </v>
+        <v>MATCH_TEAMA_ID INT(11)  comment 'A球队临时ID' , </v>
       </c>
     </row>
     <row r="66" customFormat="1" spans="1:5">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="E66" s="1" t="str">
         <f>A66&amp;" "&amp;B66&amp;" "&amp;C66&amp;" comment '"&amp;D66&amp;"' , "</f>
-        <v>MATCH_TEAMB_ID DECIMAL(10,0)  comment 'B球队临时ID' , </v>
+        <v>MATCH_TEAMB_ID INT(11)  comment 'B球队临时ID' , </v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" spans="1:5">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="E71" s="1" t="str">
         <f>A71&amp;" "&amp;B71&amp;" "&amp;C71&amp;" comment '"&amp;D71&amp;"' , "</f>
-        <v>DELSIGN DECIMAL(1,0)  comment '删除标识' , </v>
+        <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
     <row r="73" ht="18.75" spans="1:4">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="E77" s="1" t="str">
         <f>A77&amp;" "&amp;B77&amp;" "&amp;C77&amp;" comment '"&amp;D77&amp;"' , "</f>
-        <v>MM_ID DECIMAL(10,0) NOT NULL PRIMARY KEY comment '参赛人员表非空主键' , </v>
+        <v>MM_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '参赛人员表非空主键' , </v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" spans="1:5">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="E78" s="1" t="str">
         <f t="shared" ref="E78:E86" si="4">A78&amp;" "&amp;B78&amp;" "&amp;C78&amp;" comment '"&amp;D78&amp;"' , "</f>
-        <v>M_ID DECIMAL(10,0)  comment '关联比赛MID' , </v>
+        <v>M_ID INT(11)  comment '关联比赛MID' , </v>
       </c>
     </row>
     <row r="79" s="1" customFormat="1" spans="1:5">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="E79" s="1" t="str">
         <f>A79&amp;" "&amp;B79&amp;" "&amp;C79&amp;" comment '"&amp;D79&amp;"' , "</f>
-        <v>T_ID DECIMAL(10,0)  comment '报名临时球队ID' , </v>
+        <v>T_ID INT(11)  comment '报名临时球队ID' , </v>
       </c>
     </row>
     <row r="80" s="1" customFormat="1" spans="1:5">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="E80" s="1" t="str">
         <f>A80&amp;" "&amp;B80&amp;" "&amp;C80&amp;" comment '"&amp;D80&amp;"' , "</f>
-        <v>U_ID DECIMAL(10,0)  comment '关联UID' , </v>
+        <v>U_ID INT(11)  comment '关联UID' , </v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2094,7 +2094,7 @@
       </c>
       <c r="E86" s="1" t="str">
         <f>A86&amp;" "&amp;B86&amp;" "&amp;C86&amp;" comment '"&amp;D86&amp;"' , "</f>
-        <v>DELSIGN DECIMAL(1,0)  comment '删除标识' , </v>
+        <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
     <row r="88" ht="18.75" spans="1:4">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="E92" s="1" t="str">
         <f>A92&amp;" "&amp;B92&amp;" "&amp;C92&amp;" comment '"&amp;D92&amp;"' , "</f>
-        <v>D_ID DECIMAL(10,0) NOT NULL PRIMARY KEY comment '字典表非空主键' , </v>
+        <v>D_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '字典表非空主键' , </v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="E94" s="1" t="str">
         <f>A94&amp;" "&amp;B94&amp;" "&amp;C94&amp;" comment '"&amp;D94&amp;"' , "</f>
-        <v>D_TYPE DECIMAL(10,0)  comment '类型' , </v>
+        <v>D_TYPE INT(11)  comment '类型' , </v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2280,7 +2280,7 @@
       </c>
       <c r="E99" s="1" t="str">
         <f>A99&amp;" "&amp;B99&amp;" "&amp;C99&amp;" comment '"&amp;D99&amp;"' , "</f>
-        <v>DELSIGN DECIMAL(1,0)  comment '删除标识' , </v>
+        <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update t_user add nick name and eng name
</commit_message>
<xml_diff>
--- a/src/main/resources/DB.xlsx
+++ b/src/main/resources/DB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113">
   <si>
     <t>NO</t>
   </si>
@@ -79,6 +79,18 @@
     <t>用户名</t>
   </si>
   <si>
+    <t>NICK_NAME</t>
+  </si>
+  <si>
+    <t>昵称</t>
+  </si>
+  <si>
+    <t>ENG_NAME</t>
+  </si>
+  <si>
+    <t>英文名</t>
+  </si>
+  <si>
     <t>USEX</t>
   </si>
   <si>
@@ -170,6 +182,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">NOT </t>
     </r>
     <r>
@@ -397,10 +415,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -864,10 +882,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -950,7 +968,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>A5&amp;" "&amp;B5&amp;" "&amp;C5&amp;" comment '"&amp;D5&amp;"' , "</f>
+        <f t="shared" ref="E5:E10" si="0">A5&amp;" "&amp;B5&amp;" "&amp;C5&amp;" comment '"&amp;D5&amp;"' , "</f>
         <v>ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '用户表非空主键' , </v>
       </c>
     </row>
@@ -966,7 +984,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f t="shared" ref="E6" si="0">A6&amp;" "&amp;B6&amp;" "&amp;C6&amp;" comment '"&amp;D6&amp;"' , "</f>
+        <f t="shared" ref="E6" si="1">A6&amp;" "&amp;B6&amp;" "&amp;C6&amp;" comment '"&amp;D6&amp;"' , "</f>
         <v>LOGIN_NAME VARCHAR(100)  comment '用户登录名' , </v>
       </c>
     </row>
@@ -982,7 +1000,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f t="shared" ref="E7:E15" si="1">A7&amp;" "&amp;B7&amp;" "&amp;C7&amp;" comment '"&amp;D7&amp;"' , "</f>
+        <f>A7&amp;" "&amp;B7&amp;" "&amp;C7&amp;" comment '"&amp;D7&amp;"' , "</f>
         <v>LOGIN_PASSWORD VARCHAR(100)  comment '用户登录密码' , </v>
       </c>
     </row>
@@ -1007,47 +1025,47 @@
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="str">
         <f>A9&amp;" "&amp;B9&amp;" "&amp;C9&amp;" comment '"&amp;D9&amp;"' , "</f>
-        <v>USEX VARCHAR(2)  comment '用户性别' , </v>
+        <v>NICK_NAME VARCHAR(100)  comment '昵称' , </v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="str">
         <f>A10&amp;" "&amp;B10&amp;" "&amp;C10&amp;" comment '"&amp;D10&amp;"' , "</f>
-        <v>STATUS VARCHAR(2)  comment '用户激活状态' , </v>
+        <v>ENG_NAME VARCHAR(100)  comment '英文名' , </v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>A11&amp;" "&amp;B11&amp;" "&amp;C11&amp;" comment '"&amp;D11&amp;"' , "</f>
-        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
+        <f t="shared" ref="E11:E17" si="2">A11&amp;" "&amp;B11&amp;" "&amp;C11&amp;" comment '"&amp;D11&amp;"' , "</f>
+        <v>USEX VARCHAR(2)  comment '用户性别' , </v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1055,15 +1073,15 @@
         <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>A12&amp;" "&amp;B12&amp;" "&amp;C12&amp;" comment '"&amp;D12&amp;"' , "</f>
-        <v>INPUT_DATE VARCHAR(100)  comment '插入时间' , </v>
+        <v>STATUS VARCHAR(2)  comment '用户激活状态' , </v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1079,7 +1097,7 @@
       </c>
       <c r="E13" s="1" t="str">
         <f>A13&amp;" "&amp;B13&amp;" "&amp;C13&amp;" comment '"&amp;D13&amp;"' , "</f>
-        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1095,7 +1113,7 @@
       </c>
       <c r="E14" s="1" t="str">
         <f>A14&amp;" "&amp;B14&amp;" "&amp;C14&amp;" comment '"&amp;D14&amp;"' , "</f>
-        <v>UPDATE_DATE VARCHAR(100)  comment '修改时间' , </v>
+        <v>INPUT_DATE VARCHAR(100)  comment '插入时间' , </v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1103,137 +1121,137 @@
         <v>34</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>A15&amp;" "&amp;B15&amp;" "&amp;C15&amp;" comment '"&amp;D15&amp;"' , "</f>
+        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f>A16&amp;" "&amp;B16&amp;" "&amp;C16&amp;" comment '"&amp;D16&amp;"' , "</f>
+        <v>UPDATE_DATE VARCHAR(100)  comment '修改时间' , </v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f>A17&amp;" "&amp;B17&amp;" "&amp;C17&amp;" comment '"&amp;D17&amp;"' , "</f>
         <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
-    <row r="17" ht="18.75" spans="1:4">
-      <c r="A17" s="2" t="s">
+    <row r="19" ht="18.75" spans="1:4">
+      <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B19" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D19" s="4">
         <v>42269</v>
       </c>
     </row>
-    <row r="18" ht="18.75" spans="1:4">
-      <c r="A18" s="2" t="s">
+    <row r="20" ht="18.75" spans="1:4">
+      <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" ht="18.75" spans="1:5">
-      <c r="A19" s="2" t="s">
+      <c r="B20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" ht="18.75" spans="1:5">
+      <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="1" t="str">
-        <f>"drop table "&amp;B18&amp;";"</f>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="1" t="str">
+        <f>"drop table "&amp;B20&amp;";"</f>
         <v>drop table T_TEAM_FOOTBALL;</v>
       </c>
     </row>
-    <row r="20" ht="18.75" spans="1:5">
-      <c r="A20" s="2" t="s">
+    <row r="22" ht="18.75" spans="1:5">
+      <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="1" t="str">
-        <f>"create table "&amp;B18&amp;" ("</f>
+      <c r="E22" s="1" t="str">
+        <f>"create table "&amp;B20&amp;" ("</f>
         <v>create table T_TEAM_FOOTBALL (</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="1" t="str">
-        <f>A21&amp;" "&amp;B21&amp;" "&amp;C21&amp;" comment '"&amp;D21&amp;"' , "</f>
-        <v>TID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球队表非空主键' , </v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="1" t="str">
-        <f t="shared" ref="E22" si="2">A22&amp;" "&amp;B22&amp;" "&amp;C22&amp;" comment '"&amp;D22&amp;"' , "</f>
-        <v>TEAM_NAME VARCHAR(500)  comment '球队名称' , </v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>A23&amp;" "&amp;B23&amp;" "&amp;C23&amp;" comment '"&amp;D23&amp;"' , "</f>
-        <v>TEAM_CITY VARCHAR(100)  comment '球队所在城市' , </v>
+        <v>TID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球队表非空主键' , </v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>1</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E24" s="1" t="str">
-        <f>A24&amp;" "&amp;B24&amp;" "&amp;C24&amp;" comment '"&amp;D24&amp;"' , "</f>
-        <v>TEAM_CREATE_DATE DATE  comment '球队创建时间' , </v>
+        <f t="shared" ref="E24:E34" si="3">A24&amp;" "&amp;B24&amp;" "&amp;C24&amp;" comment '"&amp;D24&amp;"' , "</f>
+        <v>TEAM_NAME VARCHAR(500)  comment '球队名称' , </v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1241,15 +1259,15 @@
         <v>47</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="1" t="str">
         <f>A25&amp;" "&amp;B25&amp;" "&amp;C25&amp;" comment '"&amp;D25&amp;"' , "</f>
-        <v>TEAM_CAPTAIN INT(11)  comment '存队长的UID' , </v>
+        <v>TEAM_CITY VARCHAR(100)  comment '球队所在城市' , </v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1257,49 +1275,47 @@
         <v>49</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>A26&amp;" "&amp;B26&amp;" "&amp;C26&amp;" comment '"&amp;D26&amp;"' , "</f>
-        <v>TEAM_POINTS INT(11)  comment '球队积分' , </v>
+        <v>TEAM_CREATE_DATE DATE  comment '球队创建时间' , </v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>51</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E27" s="1" t="str">
         <f>A27&amp;" "&amp;B27&amp;" "&amp;C27&amp;" comment '"&amp;D27&amp;"' , "</f>
-        <v>STATUS INT(1) NOT NULL DEFAULT '0' comment '球队状态： 0-未审核；1-审核通过' , </v>
+        <v>TEAM_CAPTAIN INT(11)  comment '存队长的UID' , </v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="6" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E28" s="1" t="str">
         <f>A28&amp;" "&amp;B28&amp;" "&amp;C28&amp;" comment '"&amp;D28&amp;"' , "</f>
-        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
+        <v>TEAM_POINTS INT(11)  comment '球队积分' , </v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1307,15 +1323,17 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="D29" s="6" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E29" s="1" t="str">
         <f>A29&amp;" "&amp;B29&amp;" "&amp;C29&amp;" comment '"&amp;D29&amp;"' , "</f>
-        <v>INPUT_DATE DATE  comment '插入时间' , </v>
+        <v>STATUS INT(1) NOT NULL DEFAULT '0' comment '球队状态： 0-未审核；1-审核通过' , </v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1331,7 +1349,7 @@
       </c>
       <c r="E30" s="1" t="str">
         <f>A30&amp;" "&amp;B30&amp;" "&amp;C30&amp;" comment '"&amp;D30&amp;"' , "</f>
-        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1347,7 +1365,7 @@
       </c>
       <c r="E31" s="1" t="str">
         <f>A31&amp;" "&amp;B31&amp;" "&amp;C31&amp;" comment '"&amp;D31&amp;"' , "</f>
-        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+        <v>INPUT_DATE DATE  comment '插入时间' , </v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1355,105 +1373,103 @@
         <v>34</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>A32&amp;" "&amp;B32&amp;" "&amp;C32&amp;" comment '"&amp;D32&amp;"' , "</f>
+        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <f>A33&amp;" "&amp;B33&amp;" "&amp;C33&amp;" comment '"&amp;D33&amp;"' , "</f>
+        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f>A34&amp;" "&amp;B34&amp;" "&amp;C34&amp;" comment '"&amp;D34&amp;"' , "</f>
         <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
-    <row r="34" ht="18.75" spans="1:4">
-      <c r="A34" s="2" t="s">
+    <row r="36" ht="18.75" spans="1:4">
+      <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B36" s="3">
         <v>3</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D36" s="4">
         <v>42269</v>
       </c>
     </row>
-    <row r="35" ht="18.75" spans="1:4">
-      <c r="A35" s="2" t="s">
+    <row r="37" ht="18.75" spans="1:4">
+      <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" ht="18.75" spans="1:5">
-      <c r="A36" s="2" t="s">
+      <c r="B37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" ht="18.75" spans="1:5">
+      <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="1" t="str">
-        <f>"drop table "&amp;B35&amp;";"</f>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="1" t="str">
+        <f>"drop table "&amp;B37&amp;";"</f>
         <v>drop table T_TEAM_FOOTBALL_MEMBER;</v>
       </c>
     </row>
-    <row r="37" ht="18.75" spans="1:5">
-      <c r="A37" s="2" t="s">
+    <row r="39" ht="18.75" spans="1:5">
+      <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="1" t="str">
-        <f>"create table "&amp;B35&amp;" ("</f>
+      <c r="E39" s="1" t="str">
+        <f>"create table "&amp;B37&amp;" ("</f>
         <v>create table T_TEAM_FOOTBALL_MEMBER (</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="1" t="str">
-        <f>A38&amp;" "&amp;B38&amp;" "&amp;C38&amp;" comment '"&amp;D38&amp;"' , "</f>
-        <v>TM_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球队成员表非空主键' , </v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="1" t="str">
-        <f t="shared" ref="E39" si="3">A39&amp;" "&amp;B39&amp;" "&amp;C39&amp;" comment '"&amp;D39&amp;"' , "</f>
-        <v>T_ID INT(11)  comment '关联球队TID' , </v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1463,13 +1479,15 @@
       <c r="B40" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5" t="s">
+      <c r="C40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E40" s="1" t="str">
-        <f t="shared" ref="E40:E50" si="4">A40&amp;" "&amp;B40&amp;" "&amp;C40&amp;" comment '"&amp;D40&amp;"' , "</f>
-        <v>U_ID INT(11)  comment '用户ID' , </v>
+        <f>A40&amp;" "&amp;B40&amp;" "&amp;C40&amp;" comment '"&amp;D40&amp;"' , "</f>
+        <v>TM_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球队成员表非空主键' , </v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1477,47 +1495,47 @@
         <v>60</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E41" s="1" t="str">
-        <f>A41&amp;" "&amp;B41&amp;" "&amp;C41&amp;" comment '"&amp;D41&amp;"' , "</f>
-        <v>MEMBER_POSITION VARCHAR(10)  comment '在球队中职位' , </v>
+        <f t="shared" ref="E41" si="4">A41&amp;" "&amp;B41&amp;" "&amp;C41&amp;" comment '"&amp;D41&amp;"' , "</f>
+        <v>T_ID INT(11)  comment '关联球队TID' , </v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f>A42&amp;" "&amp;B42&amp;" "&amp;C42&amp;" comment '"&amp;D42&amp;"' , "</f>
-        <v>MEMBER_JOIN_DATE DATE  comment '球员加入球队时间' , </v>
+        <f t="shared" ref="E42:E52" si="5">A42&amp;" "&amp;B42&amp;" "&amp;C42&amp;" comment '"&amp;D42&amp;"' , "</f>
+        <v>U_ID INT(11)  comment '用户ID' , </v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="C43" s="5"/>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E43" s="1" t="str">
         <f>A43&amp;" "&amp;B43&amp;" "&amp;C43&amp;" comment '"&amp;D43&amp;"' , "</f>
-        <v>MEMBER_LEFT_DATE DATE  comment '球员离开球队时间' , </v>
+        <v>MEMBER_POSITION VARCHAR(10)  comment '在球队中职位' , </v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1525,15 +1543,15 @@
         <v>67</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="5" t="s">
         <v>68</v>
       </c>
       <c r="E44" s="1" t="str">
         <f>A44&amp;" "&amp;B44&amp;" "&amp;C44&amp;" comment '"&amp;D44&amp;"' , "</f>
-        <v>MEMBER_ABSENT_TIME INT(11)  comment '球员缺席次数' , </v>
+        <v>MEMBER_JOIN_DATE DATE  comment '球员加入球队时间' , </v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1549,39 +1567,39 @@
       </c>
       <c r="E45" s="1" t="str">
         <f>A45&amp;" "&amp;B45&amp;" "&amp;C45&amp;" comment '"&amp;D45&amp;"' , "</f>
-        <v>MEMBER_ABSENT_DATE DATE  comment '球员缺席时间' , </v>
+        <v>MEMBER_LEFT_DATE DATE  comment '球员离开球队时间' , </v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="6" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="E46" s="1" t="str">
         <f>A46&amp;" "&amp;B46&amp;" "&amp;C46&amp;" comment '"&amp;D46&amp;"' , "</f>
-        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
+        <v>MEMBER_ABSENT_TIME INT(11)  comment '球员缺席次数' , </v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="5" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="6" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="E47" s="1" t="str">
         <f>A47&amp;" "&amp;B47&amp;" "&amp;C47&amp;" comment '"&amp;D47&amp;"' , "</f>
-        <v>INPUT_DATE DATE  comment '插入时间' , </v>
+        <v>MEMBER_ABSENT_DATE DATE  comment '球员缺席时间' , </v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1597,7 +1615,7 @@
       </c>
       <c r="E48" s="1" t="str">
         <f>A48&amp;" "&amp;B48&amp;" "&amp;C48&amp;" comment '"&amp;D48&amp;"' , "</f>
-        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1613,7 +1631,7 @@
       </c>
       <c r="E49" s="1" t="str">
         <f>A49&amp;" "&amp;B49&amp;" "&amp;C49&amp;" comment '"&amp;D49&amp;"' , "</f>
-        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+        <v>INPUT_DATE DATE  comment '插入时间' , </v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1621,105 +1639,103 @@
         <v>34</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E50" s="1" t="str">
         <f>A50&amp;" "&amp;B50&amp;" "&amp;C50&amp;" comment '"&amp;D50&amp;"' , "</f>
+        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f>A51&amp;" "&amp;B51&amp;" "&amp;C51&amp;" comment '"&amp;D51&amp;"' , "</f>
+        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <f>A52&amp;" "&amp;B52&amp;" "&amp;C52&amp;" comment '"&amp;D52&amp;"' , "</f>
         <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
-    <row r="52" ht="18.75" spans="1:4">
-      <c r="A52" s="2" t="s">
+    <row r="54" ht="18.75" spans="1:4">
+      <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B54" s="3">
         <v>4</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D54" s="4">
         <v>42269</v>
       </c>
     </row>
-    <row r="53" ht="18.75" spans="1:4">
-      <c r="A53" s="2" t="s">
+    <row r="55" ht="18.75" spans="1:4">
+      <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="54" ht="18.75" spans="1:5">
-      <c r="A54" s="2" t="s">
+      <c r="B55" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" ht="18.75" spans="1:5">
+      <c r="A56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="1" t="str">
-        <f>"drop table "&amp;B53&amp;";"</f>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="1" t="str">
+        <f>"drop table "&amp;B55&amp;";"</f>
         <v>drop table T_MATCH_FOOTBALL;</v>
       </c>
     </row>
-    <row r="55" ht="18.75" spans="1:5">
-      <c r="A55" s="2" t="s">
+    <row r="57" ht="18.75" spans="1:5">
+      <c r="A57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="1" t="str">
-        <f>"create table "&amp;B53&amp;" ("</f>
+      <c r="E57" s="1" t="str">
+        <f>"create table "&amp;B55&amp;" ("</f>
         <v>create table T_MATCH_FOOTBALL (</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E56" s="1" t="str">
-        <f>A56&amp;" "&amp;B56&amp;" "&amp;C56&amp;" comment '"&amp;D56&amp;"' , "</f>
-        <v>M_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球比赛表非空主键' , </v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E57" s="1" t="str">
-        <f t="shared" ref="E57" si="5">A57&amp;" "&amp;B57&amp;" "&amp;C57&amp;" comment '"&amp;D57&amp;"' , "</f>
-        <v>MATCH_DATE DATE  comment '比赛日期' , </v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1727,15 +1743,17 @@
         <v>76</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C58" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D58" s="5" t="s">
         <v>77</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f t="shared" ref="E58:E71" si="6">A58&amp;" "&amp;B58&amp;" "&amp;C58&amp;" comment '"&amp;D58&amp;"' , "</f>
-        <v>MATCH_ADDRESS VARCHAR(500)  comment '球队比赛地点' , </v>
+        <f>A58&amp;" "&amp;B58&amp;" "&amp;C58&amp;" comment '"&amp;D58&amp;"' , "</f>
+        <v>M_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '足球比赛表非空主键' , </v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1743,15 +1761,15 @@
         <v>78</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E59" s="1" t="str">
-        <f>A59&amp;" "&amp;B59&amp;" "&amp;C59&amp;" comment '"&amp;D59&amp;"' , "</f>
-        <v>MATCH_ORGANIZER INT(11)  comment '组织者UID' , </v>
+        <f t="shared" ref="E59" si="6">A59&amp;" "&amp;B59&amp;" "&amp;C59&amp;" comment '"&amp;D59&amp;"' , "</f>
+        <v>MATCH_DATE DATE  comment '比赛日期' , </v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1759,15 +1777,15 @@
         <v>80</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C60" s="5"/>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="5" t="s">
         <v>81</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f>A60&amp;" "&amp;B60&amp;" "&amp;C60&amp;" comment '"&amp;D60&amp;"' , "</f>
-        <v>MATCH_KEEPER_MEMBERS INT(11)  comment '守门员人数' , </v>
+        <f t="shared" ref="E60:E73" si="7">A60&amp;" "&amp;B60&amp;" "&amp;C60&amp;" comment '"&amp;D60&amp;"' , "</f>
+        <v>MATCH_ADDRESS VARCHAR(500)  comment '球队比赛地点' , </v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1778,12 +1796,12 @@
         <v>11</v>
       </c>
       <c r="C61" s="5"/>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="5" t="s">
         <v>83</v>
       </c>
       <c r="E61" s="1" t="str">
         <f>A61&amp;" "&amp;B61&amp;" "&amp;C61&amp;" comment '"&amp;D61&amp;"' , "</f>
-        <v>MATCH_DEFENDER_MEMBERS INT(11)  comment '后卫人数' , </v>
+        <v>MATCH_ORGANIZER INT(11)  comment '组织者UID' , </v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1799,7 +1817,7 @@
       </c>
       <c r="E62" s="1" t="str">
         <f>A62&amp;" "&amp;B62&amp;" "&amp;C62&amp;" comment '"&amp;D62&amp;"' , "</f>
-        <v>MATCH_MIDFIELDER_MEMBERS INT(11)  comment '中场人数' , </v>
+        <v>MATCH_KEEPER_MEMBERS INT(11)  comment '守门员人数' , </v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1815,10 +1833,10 @@
       </c>
       <c r="E63" s="1" t="str">
         <f>A63&amp;" "&amp;B63&amp;" "&amp;C63&amp;" comment '"&amp;D63&amp;"' , "</f>
-        <v>MATCH_STRIKER_MEMBERS INT(11)  comment '前锋人数' , </v>
-      </c>
-    </row>
-    <row r="64" customFormat="1" spans="1:5">
+        <v>MATCH_DEFENDER_MEMBERS INT(11)  comment '后卫人数' , </v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="5" t="s">
         <v>88</v>
       </c>
@@ -1831,10 +1849,10 @@
       </c>
       <c r="E64" s="1" t="str">
         <f>A64&amp;" "&amp;B64&amp;" "&amp;C64&amp;" comment '"&amp;D64&amp;"' , "</f>
-        <v>MATCH_REFEREE_MEMBERS INT(11)  comment '裁判人数' , </v>
-      </c>
-    </row>
-    <row r="65" customFormat="1" spans="1:5">
+        <v>MATCH_MIDFIELDER_MEMBERS INT(11)  comment '中场人数' , </v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="5" t="s">
         <v>90</v>
       </c>
@@ -1847,7 +1865,7 @@
       </c>
       <c r="E65" s="1" t="str">
         <f>A65&amp;" "&amp;B65&amp;" "&amp;C65&amp;" comment '"&amp;D65&amp;"' , "</f>
-        <v>MATCH_TEAMA_ID INT(11)  comment 'A球队临时ID' , </v>
+        <v>MATCH_STRIKER_MEMBERS INT(11)  comment '前锋人数' , </v>
       </c>
     </row>
     <row r="66" customFormat="1" spans="1:5">
@@ -1863,39 +1881,39 @@
       </c>
       <c r="E66" s="1" t="str">
         <f>A66&amp;" "&amp;B66&amp;" "&amp;C66&amp;" comment '"&amp;D66&amp;"' , "</f>
-        <v>MATCH_TEAMB_ID INT(11)  comment 'B球队临时ID' , </v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>MATCH_REFEREE_MEMBERS INT(11)  comment '裁判人数' , </v>
+      </c>
+    </row>
+    <row r="67" customFormat="1" spans="1:5">
       <c r="A67" s="5" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="6" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="E67" s="1" t="str">
         <f>A67&amp;" "&amp;B67&amp;" "&amp;C67&amp;" comment '"&amp;D67&amp;"' , "</f>
-        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>MATCH_TEAMA_ID INT(11)  comment 'A球队临时ID' , </v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" spans="1:5">
       <c r="A68" s="5" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="6" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="E68" s="1" t="str">
         <f>A68&amp;" "&amp;B68&amp;" "&amp;C68&amp;" comment '"&amp;D68&amp;"' , "</f>
-        <v>INPUT_DATE DATE  comment '插入时间' , </v>
+        <v>MATCH_TEAMB_ID INT(11)  comment 'B球队临时ID' , </v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1911,7 +1929,7 @@
       </c>
       <c r="E69" s="1" t="str">
         <f>A69&amp;" "&amp;B69&amp;" "&amp;C69&amp;" comment '"&amp;D69&amp;"' , "</f>
-        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1927,7 +1945,7 @@
       </c>
       <c r="E70" s="1" t="str">
         <f>A70&amp;" "&amp;B70&amp;" "&amp;C70&amp;" comment '"&amp;D70&amp;"' , "</f>
-        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+        <v>INPUT_DATE DATE  comment '插入时间' , </v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1935,185 +1953,185 @@
         <v>34</v>
       </c>
       <c r="B71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E71" s="1" t="str">
         <f>A71&amp;" "&amp;B71&amp;" "&amp;C71&amp;" comment '"&amp;D71&amp;"' , "</f>
+        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E72" s="1" t="str">
+        <f>A72&amp;" "&amp;B72&amp;" "&amp;C72&amp;" comment '"&amp;D72&amp;"' , "</f>
+        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73" s="1" t="str">
+        <f>A73&amp;" "&amp;B73&amp;" "&amp;C73&amp;" comment '"&amp;D73&amp;"' , "</f>
         <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
-    <row r="73" ht="18.75" spans="1:4">
-      <c r="A73" s="2" t="s">
+    <row r="75" ht="18.75" spans="1:4">
+      <c r="A75" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B75" s="3">
         <v>5</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D75" s="4">
         <v>42269</v>
       </c>
     </row>
-    <row r="74" ht="18.75" spans="1:4">
-      <c r="A74" s="2" t="s">
+    <row r="76" ht="18.75" spans="1:4">
+      <c r="A76" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-    </row>
-    <row r="75" ht="18.75" spans="1:5">
-      <c r="A75" s="2" t="s">
+      <c r="B76" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" ht="18.75" spans="1:5">
+      <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B77" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="1" t="str">
-        <f>"drop table "&amp;B74&amp;";"</f>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="1" t="str">
+        <f>"drop table "&amp;B76&amp;";"</f>
         <v>drop table T_MATCH_FOOTBALL_MEMBER;</v>
       </c>
     </row>
-    <row r="76" ht="18.75" spans="1:5">
-      <c r="A76" s="2" t="s">
+    <row r="78" ht="18.75" spans="1:5">
+      <c r="A78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E76" s="1" t="str">
-        <f>"create table "&amp;B74&amp;" ("</f>
+      <c r="E78" s="1" t="str">
+        <f>"create table "&amp;B76&amp;" ("</f>
         <v>create table T_MATCH_FOOTBALL_MEMBER (</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E77" s="1" t="str">
-        <f>A77&amp;" "&amp;B77&amp;" "&amp;C77&amp;" comment '"&amp;D77&amp;"' , "</f>
-        <v>MM_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '参赛人员表非空主键' , </v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E78" s="1" t="str">
-        <f t="shared" ref="E78" si="7">A78&amp;" "&amp;B78&amp;" "&amp;C78&amp;" comment '"&amp;D78&amp;"' , "</f>
-        <v>M_ID INT(11)  comment '关联比赛MID' , </v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="5" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D79" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E79" s="1" t="str">
-        <f t="shared" ref="E79:E86" si="8">A79&amp;" "&amp;B79&amp;" "&amp;C79&amp;" comment '"&amp;D79&amp;"' , "</f>
-        <v>T_ID INT(11)  comment '报名临时球队ID' , </v>
+        <f>A79&amp;" "&amp;B79&amp;" "&amp;C79&amp;" comment '"&amp;D79&amp;"' , "</f>
+        <v>MM_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '参赛人员表非空主键' , </v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="5" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E80" s="1" t="str">
-        <f>A80&amp;" "&amp;B80&amp;" "&amp;C80&amp;" comment '"&amp;D80&amp;"' , "</f>
-        <v>U_ID INT(11)  comment '关联UID' , </v>
+        <f t="shared" ref="E80" si="8">A80&amp;" "&amp;B80&amp;" "&amp;C80&amp;" comment '"&amp;D80&amp;"' , "</f>
+        <v>M_ID INT(11)  comment '关联比赛MID' , </v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="5" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E81" s="1" t="str">
-        <f>A81&amp;" "&amp;B81&amp;" "&amp;C81&amp;" comment '"&amp;D81&amp;"' , "</f>
-        <v>MATCH_MEMBER_POSITION VARCHAR(100)  comment '报名者踢球的位置' , </v>
+        <f t="shared" ref="E81:E88" si="9">A81&amp;" "&amp;B81&amp;" "&amp;C81&amp;" comment '"&amp;D81&amp;"' , "</f>
+        <v>T_ID INT(11)  comment '报名临时球队ID' , </v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="5" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C82" s="5"/>
-      <c r="D82" s="6" t="s">
-        <v>27</v>
+      <c r="D82" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="E82" s="1" t="str">
         <f>A82&amp;" "&amp;B82&amp;" "&amp;C82&amp;" comment '"&amp;D82&amp;"' , "</f>
-        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
+        <v>U_ID INT(11)  comment '关联UID' , </v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="5" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C83" s="5"/>
-      <c r="D83" s="6" t="s">
-        <v>29</v>
+      <c r="D83" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="E83" s="1" t="str">
         <f>A83&amp;" "&amp;B83&amp;" "&amp;C83&amp;" comment '"&amp;D83&amp;"' , "</f>
-        <v>INPUT_DATE DATE  comment '插入时间' , </v>
+        <v>MATCH_MEMBER_POSITION VARCHAR(100)  comment '报名者踢球的位置' , </v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2129,7 +2147,7 @@
       </c>
       <c r="E84" s="1" t="str">
         <f>A84&amp;" "&amp;B84&amp;" "&amp;C84&amp;" comment '"&amp;D84&amp;"' , "</f>
-        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2145,7 +2163,7 @@
       </c>
       <c r="E85" s="1" t="str">
         <f>A85&amp;" "&amp;B85&amp;" "&amp;C85&amp;" comment '"&amp;D85&amp;"' , "</f>
-        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+        <v>INPUT_DATE DATE  comment '插入时间' , </v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2153,105 +2171,103 @@
         <v>34</v>
       </c>
       <c r="B86" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E86" s="1" t="str">
         <f>A86&amp;" "&amp;B86&amp;" "&amp;C86&amp;" comment '"&amp;D86&amp;"' , "</f>
+        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E87" s="1" t="str">
+        <f>A87&amp;" "&amp;B87&amp;" "&amp;C87&amp;" comment '"&amp;D87&amp;"' , "</f>
+        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E88" s="1" t="str">
+        <f>A88&amp;" "&amp;B88&amp;" "&amp;C88&amp;" comment '"&amp;D88&amp;"' , "</f>
         <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>
-    <row r="88" ht="18.75" spans="1:4">
-      <c r="A88" s="2" t="s">
+    <row r="90" ht="18.75" spans="1:4">
+      <c r="A90" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B90" s="3">
         <v>5</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D90" s="4">
         <v>42269</v>
       </c>
     </row>
-    <row r="89" ht="18.75" spans="1:4">
-      <c r="A89" s="2" t="s">
+    <row r="91" ht="18.75" spans="1:4">
+      <c r="A91" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-    </row>
-    <row r="90" ht="18.75" spans="1:5">
-      <c r="A90" s="2" t="s">
+      <c r="B91" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" ht="18.75" spans="1:5">
+      <c r="A92" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B92" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="1" t="str">
-        <f>"drop table "&amp;B89&amp;";"</f>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="1" t="str">
+        <f>"drop table "&amp;B91&amp;";"</f>
         <v>drop table T_DICTIONARY;</v>
       </c>
     </row>
-    <row r="91" ht="18.75" spans="1:5">
-      <c r="A91" s="2" t="s">
+    <row r="93" ht="18.75" spans="1:5">
+      <c r="A93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E91" s="1" t="str">
-        <f>"create table "&amp;B89&amp;" ("</f>
+      <c r="E93" s="1" t="str">
+        <f>"create table "&amp;B91&amp;" ("</f>
         <v>create table T_DICTIONARY (</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E92" s="1" t="str">
-        <f>A92&amp;" "&amp;B92&amp;" "&amp;C92&amp;" comment '"&amp;D92&amp;"' , "</f>
-        <v>D_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '字典表非空主键' , </v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E93" s="1" t="str">
-        <f t="shared" ref="E93" si="9">A93&amp;" "&amp;B93&amp;" "&amp;C93&amp;" comment '"&amp;D93&amp;"' , "</f>
-        <v>D_NAMME VARCHAR(500)  comment '名称' , </v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2261,45 +2277,47 @@
       <c r="B94" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D94" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E94" s="1" t="str">
-        <f t="shared" ref="E94:E99" si="10">A94&amp;" "&amp;B94&amp;" "&amp;C94&amp;" comment '"&amp;D94&amp;"' , "</f>
-        <v>D_TYPE INT(11)  comment '类型' , </v>
+        <f>A94&amp;" "&amp;B94&amp;" "&amp;C94&amp;" comment '"&amp;D94&amp;"' , "</f>
+        <v>D_ID INT(11) NOT NULL PRIMARY KEY AUTO_INCREMENT comment '字典表非空主键' , </v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="5" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C95" s="5"/>
-      <c r="D95" s="6" t="s">
-        <v>27</v>
+      <c r="D95" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="E95" s="1" t="str">
-        <f>A95&amp;" "&amp;B95&amp;" "&amp;C95&amp;" comment '"&amp;D95&amp;"' , "</f>
-        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
+        <f t="shared" ref="E95" si="10">A95&amp;" "&amp;B95&amp;" "&amp;C95&amp;" comment '"&amp;D95&amp;"' , "</f>
+        <v>D_NAMME VARCHAR(500)  comment '名称' , </v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="5" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C96" s="5"/>
-      <c r="D96" s="6" t="s">
-        <v>29</v>
+      <c r="D96" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="E96" s="1" t="str">
-        <f>A96&amp;" "&amp;B96&amp;" "&amp;C96&amp;" comment '"&amp;D96&amp;"' , "</f>
-        <v>INPUT_DATE DATE  comment '插入时间' , </v>
+        <f t="shared" ref="E96:E101" si="11">A96&amp;" "&amp;B96&amp;" "&amp;C96&amp;" comment '"&amp;D96&amp;"' , "</f>
+        <v>D_TYPE INT(11)  comment '类型' , </v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2315,7 +2333,7 @@
       </c>
       <c r="E97" s="1" t="str">
         <f>A97&amp;" "&amp;B97&amp;" "&amp;C97&amp;" comment '"&amp;D97&amp;"' , "</f>
-        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+        <v>INPUT_NAME VARCHAR(100)  comment '插入人' , </v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2331,7 +2349,7 @@
       </c>
       <c r="E98" s="1" t="str">
         <f>A98&amp;" "&amp;B98&amp;" "&amp;C98&amp;" comment '"&amp;D98&amp;"' , "</f>
-        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+        <v>INPUT_DATE DATE  comment '插入时间' , </v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2339,14 +2357,46 @@
         <v>34</v>
       </c>
       <c r="B99" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E99" s="1" t="str">
         <f>A99&amp;" "&amp;B99&amp;" "&amp;C99&amp;" comment '"&amp;D99&amp;"' , "</f>
+        <v>UPDATE_NAME VARCHAR(100)  comment '修改人' , </v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E100" s="1" t="str">
+        <f>A100&amp;" "&amp;B100&amp;" "&amp;C100&amp;" comment '"&amp;D100&amp;"' , "</f>
+        <v>UPDATE_DATE DATE  comment '修改时间' , </v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E101" s="1" t="str">
+        <f>A101&amp;" "&amp;B101&amp;" "&amp;C101&amp;" comment '"&amp;D101&amp;"' , "</f>
         <v>DELSIGN INT(1)  comment '删除标识' , </v>
       </c>
     </row>

</xml_diff>